<commit_message>
Especificando funcionamento do HD
</commit_message>
<xml_diff>
--- a/src/LAB 05 - Guilherme - Danilo - Giovanni.xlsx
+++ b/src/LAB 05 - Guilherme - Danilo - Giovanni.xlsx
@@ -5,16 +5,18 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\documentos\fei\so\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\documentos\fei\so\hd_virtual\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="4"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
-    <sheet name="EXEMPLOS" sheetId="2" r:id="rId2"/>
-    <sheet name="Planilha3" sheetId="3" r:id="rId3"/>
+    <sheet name="Descrição dos blocos" sheetId="1" r:id="rId1"/>
+    <sheet name="Exemplo dos blocos" sheetId="2" r:id="rId2"/>
+    <sheet name="Cenário 1" sheetId="3" r:id="rId3"/>
+    <sheet name="Cenário 2" sheetId="4" r:id="rId4"/>
+    <sheet name="Cenário 3" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="74">
   <si>
     <t>FLAG</t>
   </si>
@@ -67,9 +69,6 @@
     <t>BIT</t>
   </si>
   <si>
-    <t>DELETADO</t>
-  </si>
-  <si>
     <t>TEM NOME</t>
   </si>
   <si>
@@ -224,13 +223,40 @@
   </si>
   <si>
     <t>header</t>
+  </si>
+  <si>
+    <t>41 72 71 75 69 76 6f 5f 44</t>
+  </si>
+  <si>
+    <t>44 44 44 44 44 44 44 44 44 44 44 44 44 44 44 44 44 44 44 44 44 44 44 44 44 44 44 44 44 44 44 44 44 44 44 44 44 44 44 44 44 44 44 44</t>
+  </si>
+  <si>
+    <t>41 72 71 75 69 76 6f 5f 45</t>
+  </si>
+  <si>
+    <t>0002 0003 0004 0005</t>
+  </si>
+  <si>
+    <t>0006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 45 </t>
+  </si>
+  <si>
+    <t>80</t>
+  </si>
+  <si>
+    <t>45 45 45 45 45 45 45 45 45 45 45 45</t>
+  </si>
+  <si>
+    <t>OCUPADO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -264,6 +290,13 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -386,7 +419,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -403,50 +436,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -467,6 +464,44 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -475,12 +510,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -490,8 +519,24 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="40% - Ênfase1" xfId="1" builtinId="31"/>
@@ -776,7 +821,7 @@
   <dimension ref="A1:P37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -793,18 +838,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="I1" s="10" t="s">
+      <c r="B1" s="29"/>
+      <c r="I1" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="10"/>
-      <c r="O1" s="10" t="s">
+      <c r="J1" s="30"/>
+      <c r="O1" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="10"/>
+      <c r="P1" s="30"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -830,7 +875,7 @@
       <c r="A3" s="2">
         <v>0</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="27" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="1"/>
@@ -843,7 +888,7 @@
       <c r="O3" s="2">
         <v>0</v>
       </c>
-      <c r="P3" s="11" t="s">
+      <c r="P3" s="27" t="s">
         <v>5</v>
       </c>
     </row>
@@ -851,7 +896,7 @@
       <c r="A4" s="2">
         <v>1</v>
       </c>
-      <c r="B4" s="11"/>
+      <c r="B4" s="27"/>
       <c r="C4" s="1"/>
       <c r="I4" s="4">
         <v>1</v>
@@ -862,13 +907,13 @@
       <c r="O4" s="2">
         <v>1</v>
       </c>
-      <c r="P4" s="11"/>
+      <c r="P4" s="27"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>2</v>
       </c>
-      <c r="B5" s="11"/>
+      <c r="B5" s="27"/>
       <c r="I5" s="4">
         <v>2</v>
       </c>
@@ -878,13 +923,13 @@
       <c r="O5" s="2">
         <v>2</v>
       </c>
-      <c r="P5" s="11"/>
+      <c r="P5" s="27"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>3</v>
       </c>
-      <c r="B6" s="11"/>
+      <c r="B6" s="27"/>
       <c r="I6" s="4">
         <v>3</v>
       </c>
@@ -894,7 +939,7 @@
       <c r="O6" s="2">
         <v>3</v>
       </c>
-      <c r="P6" s="11"/>
+      <c r="P6" s="27"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
@@ -904,12 +949,12 @@
         <v>0</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="E7" s="10"/>
+      <c r="E7" s="30"/>
       <c r="I7" s="4">
         <v>4</v>
       </c>
@@ -927,7 +972,7 @@
       <c r="A8" s="2">
         <v>5</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="28" t="s">
         <v>1</v>
       </c>
       <c r="D8" s="2" t="s">
@@ -947,20 +992,20 @@
       <c r="O8" s="2">
         <v>5</v>
       </c>
-      <c r="P8" s="11" t="s">
-        <v>16</v>
+      <c r="P8" s="27" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>6</v>
       </c>
-      <c r="B9" s="13"/>
+      <c r="B9" s="28"/>
       <c r="D9" s="2">
         <v>0</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>13</v>
+        <v>73</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="9"/>
@@ -973,18 +1018,18 @@
       <c r="O9" s="2">
         <v>6</v>
       </c>
-      <c r="P9" s="11"/>
+      <c r="P9" s="27"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>7</v>
       </c>
-      <c r="B10" s="13"/>
+      <c r="B10" s="28"/>
       <c r="D10" s="2">
         <v>1</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F10" s="7"/>
       <c r="G10" s="9"/>
@@ -997,18 +1042,18 @@
       <c r="O10" s="2">
         <v>7</v>
       </c>
-      <c r="P10" s="11"/>
+      <c r="P10" s="27"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="13"/>
+      <c r="B11" s="28"/>
       <c r="D11" s="2">
         <v>2</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F11" s="7"/>
       <c r="G11" s="9"/>
@@ -1021,13 +1066,13 @@
       <c r="O11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="P11" s="11"/>
+      <c r="P11" s="27"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="13"/>
+      <c r="B12" s="28"/>
       <c r="D12" s="2">
         <v>3</v>
       </c>
@@ -1043,13 +1088,13 @@
       <c r="O12" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="P12" s="11"/>
+      <c r="P12" s="27"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="13"/>
+      <c r="B13" s="28"/>
       <c r="D13" s="2">
         <v>4</v>
       </c>
@@ -1065,13 +1110,13 @@
       <c r="O13" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="P13" s="11"/>
+      <c r="P13" s="27"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>31</v>
       </c>
-      <c r="B14" s="13"/>
+      <c r="B14" s="28"/>
       <c r="D14" s="2">
         <v>5</v>
       </c>
@@ -1087,13 +1132,13 @@
       <c r="O14" s="2">
         <v>31</v>
       </c>
-      <c r="P14" s="11"/>
+      <c r="P14" s="27"/>
     </row>
     <row r="15" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>32</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="28" t="s">
         <v>4</v>
       </c>
       <c r="D15" s="2">
@@ -1111,15 +1156,15 @@
       <c r="O15" s="2">
         <v>32</v>
       </c>
-      <c r="P15" s="12" t="s">
-        <v>17</v>
+      <c r="P15" s="31" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>34</v>
       </c>
-      <c r="B16" s="13"/>
+      <c r="B16" s="28"/>
       <c r="D16" s="2">
         <v>7</v>
       </c>
@@ -1135,13 +1180,13 @@
       <c r="O16" s="2">
         <v>34</v>
       </c>
-      <c r="P16" s="12"/>
+      <c r="P16" s="31"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>35</v>
       </c>
-      <c r="B17" s="13"/>
+      <c r="B17" s="28"/>
       <c r="I17" s="4">
         <v>14</v>
       </c>
@@ -1151,13 +1196,13 @@
       <c r="O17" s="2">
         <v>35</v>
       </c>
-      <c r="P17" s="12"/>
+      <c r="P17" s="31"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>36</v>
       </c>
-      <c r="B18" s="13"/>
+      <c r="B18" s="28"/>
       <c r="I18" s="4">
         <v>15</v>
       </c>
@@ -1167,13 +1212,13 @@
       <c r="O18" s="2">
         <v>36</v>
       </c>
-      <c r="P18" s="12"/>
+      <c r="P18" s="31"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>37</v>
       </c>
-      <c r="B19" s="13"/>
+      <c r="B19" s="28"/>
       <c r="I19" s="4">
         <v>16</v>
       </c>
@@ -1183,13 +1228,13 @@
       <c r="O19" s="2">
         <v>37</v>
       </c>
-      <c r="P19" s="12"/>
+      <c r="P19" s="31"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>38</v>
       </c>
-      <c r="B20" s="13"/>
+      <c r="B20" s="28"/>
       <c r="I20" s="4">
         <v>17</v>
       </c>
@@ -1199,13 +1244,13 @@
       <c r="O20" s="2">
         <v>38</v>
       </c>
-      <c r="P20" s="12"/>
+      <c r="P20" s="31"/>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>39</v>
       </c>
-      <c r="B21" s="13"/>
+      <c r="B21" s="28"/>
       <c r="I21" s="4">
         <v>18</v>
       </c>
@@ -1215,14 +1260,14 @@
       <c r="O21" s="2">
         <v>39</v>
       </c>
-      <c r="P21" s="12"/>
+      <c r="P21" s="31"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>40</v>
       </c>
-      <c r="B22" s="13"/>
-      <c r="D22" s="15"/>
+      <c r="B22" s="28"/>
+      <c r="D22" s="10"/>
       <c r="I22" s="4">
         <v>19</v>
       </c>
@@ -1232,13 +1277,13 @@
       <c r="O22" s="2">
         <v>40</v>
       </c>
-      <c r="P22" s="12"/>
+      <c r="P22" s="31"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>41</v>
       </c>
-      <c r="B23" s="13"/>
+      <c r="B23" s="28"/>
       <c r="I23" s="4">
         <v>20</v>
       </c>
@@ -1248,13 +1293,13 @@
       <c r="O23" s="2">
         <v>41</v>
       </c>
-      <c r="P23" s="12"/>
+      <c r="P23" s="31"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>42</v>
       </c>
-      <c r="B24" s="13"/>
+      <c r="B24" s="28"/>
       <c r="I24" s="4">
         <v>21</v>
       </c>
@@ -1264,13 +1309,13 @@
       <c r="O24" s="2">
         <v>42</v>
       </c>
-      <c r="P24" s="12"/>
+      <c r="P24" s="31"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>43</v>
       </c>
-      <c r="B25" s="13"/>
+      <c r="B25" s="28"/>
       <c r="I25" s="4">
         <v>22</v>
       </c>
@@ -1280,13 +1325,13 @@
       <c r="O25" s="2">
         <v>43</v>
       </c>
-      <c r="P25" s="12"/>
+      <c r="P25" s="31"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>44</v>
       </c>
-      <c r="B26" s="13"/>
+      <c r="B26" s="28"/>
       <c r="I26" s="4">
         <v>23</v>
       </c>
@@ -1296,13 +1341,13 @@
       <c r="O26" s="2">
         <v>44</v>
       </c>
-      <c r="P26" s="12"/>
+      <c r="P26" s="31"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>45</v>
       </c>
-      <c r="B27" s="13"/>
+      <c r="B27" s="28"/>
       <c r="I27" s="4">
         <v>24</v>
       </c>
@@ -1312,13 +1357,13 @@
       <c r="O27" s="2">
         <v>45</v>
       </c>
-      <c r="P27" s="12"/>
+      <c r="P27" s="31"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>46</v>
       </c>
-      <c r="B28" s="13"/>
+      <c r="B28" s="28"/>
       <c r="I28" s="4">
         <v>25</v>
       </c>
@@ -1328,13 +1373,13 @@
       <c r="O28" s="2">
         <v>46</v>
       </c>
-      <c r="P28" s="12"/>
+      <c r="P28" s="31"/>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>47</v>
       </c>
-      <c r="B29" s="13"/>
+      <c r="B29" s="28"/>
       <c r="I29" s="4">
         <v>26</v>
       </c>
@@ -1344,13 +1389,13 @@
       <c r="O29" s="2">
         <v>47</v>
       </c>
-      <c r="P29" s="12"/>
+      <c r="P29" s="31"/>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>48</v>
       </c>
-      <c r="B30" s="13"/>
+      <c r="B30" s="28"/>
       <c r="I30" s="4">
         <v>27</v>
       </c>
@@ -1360,13 +1405,13 @@
       <c r="O30" s="2">
         <v>48</v>
       </c>
-      <c r="P30" s="12"/>
+      <c r="P30" s="31"/>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B31" s="13"/>
+      <c r="B31" s="28"/>
       <c r="I31" s="4">
         <v>28</v>
       </c>
@@ -1376,13 +1421,13 @@
       <c r="O31" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="P31" s="12"/>
+      <c r="P31" s="31"/>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B32" s="13"/>
+      <c r="B32" s="28"/>
       <c r="I32" s="4">
         <v>29</v>
       </c>
@@ -1392,13 +1437,13 @@
       <c r="O32" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="P32" s="12"/>
+      <c r="P32" s="31"/>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B33" s="13"/>
+      <c r="B33" s="28"/>
       <c r="I33" s="4">
         <v>30</v>
       </c>
@@ -1408,13 +1453,13 @@
       <c r="O33" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="P33" s="12"/>
+      <c r="P33" s="31"/>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>127</v>
       </c>
-      <c r="B34" s="13"/>
+      <c r="B34" s="28"/>
       <c r="I34" s="4">
         <v>31</v>
       </c>
@@ -1424,7 +1469,7 @@
       <c r="O34" s="2">
         <v>127</v>
       </c>
-      <c r="P34" s="12"/>
+      <c r="P34" s="31"/>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="I35" s="5" t="s">
@@ -1452,16 +1497,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="P3:P6"/>
+    <mergeCell ref="P8:P14"/>
+    <mergeCell ref="P15:P34"/>
+    <mergeCell ref="D7:E7"/>
     <mergeCell ref="B3:B6"/>
     <mergeCell ref="B8:B14"/>
     <mergeCell ref="B15:B34"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="I1:J1"/>
-    <mergeCell ref="O1:P1"/>
-    <mergeCell ref="P3:P6"/>
-    <mergeCell ref="P8:P14"/>
-    <mergeCell ref="P15:P34"/>
-    <mergeCell ref="D7:E7"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1473,493 +1518,493 @@
   <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="J36" sqref="J36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="19"/>
-    <col min="2" max="2" width="11" style="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="19"/>
-    <col min="6" max="6" width="11" style="19" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="13"/>
+    <col min="2" max="2" width="11" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="13"/>
+    <col min="6" max="6" width="11" style="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="36"/>
+      <c r="E1" s="43" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="43"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="12">
+        <v>0</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="12">
+        <v>0</v>
+      </c>
+      <c r="F3" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="E1" s="16" t="s">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="12">
+        <v>1</v>
+      </c>
+      <c r="B4" s="33"/>
+      <c r="E4" s="12">
+        <v>1</v>
+      </c>
+      <c r="F4" s="44"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="12">
+        <v>2</v>
+      </c>
+      <c r="B5" s="33"/>
+      <c r="E5" s="12">
+        <v>2</v>
+      </c>
+      <c r="F5" s="44"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="12">
+        <v>3</v>
+      </c>
+      <c r="B6" s="33"/>
+      <c r="E6" s="12">
+        <v>3</v>
+      </c>
+      <c r="F6" s="44"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="12">
+        <v>4</v>
+      </c>
+      <c r="B7" s="33"/>
+      <c r="E7" s="12">
+        <v>4</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H7" s="20" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="12">
+        <v>5</v>
+      </c>
+      <c r="B8" s="33"/>
+      <c r="E8" s="15">
+        <v>5</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="H8" s="37" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="12">
+        <v>6</v>
+      </c>
+      <c r="B9" s="33"/>
+      <c r="E9" s="15">
+        <v>6</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="G9" s="21">
+        <v>1</v>
+      </c>
+      <c r="H9" s="38"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="12">
+        <v>7</v>
+      </c>
+      <c r="B10" s="33"/>
+      <c r="E10" s="15">
+        <v>7</v>
+      </c>
+      <c r="F10" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" s="21"/>
+      <c r="H10" s="38"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="12">
+        <v>8</v>
+      </c>
+      <c r="B11" s="33"/>
+      <c r="E11" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" s="21"/>
+      <c r="H11" s="38"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="12">
+        <v>9</v>
+      </c>
+      <c r="B12" s="33"/>
+      <c r="E12" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="G12" s="21"/>
+      <c r="H12" s="38"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="12">
+        <v>10</v>
+      </c>
+      <c r="B13" s="33"/>
+      <c r="E13" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="G13" s="21"/>
+      <c r="H13" s="38"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="12">
+        <v>11</v>
+      </c>
+      <c r="B14" s="33"/>
+      <c r="E14" s="15">
+        <v>31</v>
+      </c>
+      <c r="F14" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="G14" s="22"/>
+      <c r="H14" s="39"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="33"/>
+      <c r="E15" s="15">
+        <v>32</v>
+      </c>
+      <c r="F15" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="G15" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="H15" s="40" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="33"/>
+      <c r="E16" s="15">
+        <v>34</v>
+      </c>
+      <c r="F16" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="G16" s="24">
+        <v>1</v>
+      </c>
+      <c r="H16" s="41"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="33"/>
+      <c r="E17" s="15">
+        <v>35</v>
+      </c>
+      <c r="F17" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="G17" s="21"/>
+      <c r="H17" s="41"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="34"/>
+      <c r="E18" s="15">
+        <v>36</v>
+      </c>
+      <c r="F18" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="G18" s="21"/>
+      <c r="H18" s="41"/>
+    </row>
+    <row r="19" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="E19" s="15">
+        <v>37</v>
+      </c>
+      <c r="F19" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="G19" s="21"/>
+      <c r="H19" s="41"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="33"/>
+      <c r="E20" s="15">
+        <v>38</v>
+      </c>
+      <c r="F20" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="G20" s="21"/>
+      <c r="H20" s="41"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="33"/>
+      <c r="E21" s="15">
+        <v>39</v>
+      </c>
+      <c r="F21" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="G21" s="21"/>
+      <c r="H21" s="41"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" s="33"/>
+      <c r="E22" s="15">
+        <v>40</v>
+      </c>
+      <c r="F22" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="G22" s="21"/>
+      <c r="H22" s="41"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="33"/>
+      <c r="E23" s="15">
+        <v>41</v>
+      </c>
+      <c r="F23" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="G23" s="21"/>
+      <c r="H23" s="41"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" s="33"/>
+      <c r="E24" s="15">
+        <v>42</v>
+      </c>
+      <c r="F24" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="G24" s="21"/>
+      <c r="H24" s="41"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" s="33"/>
+      <c r="E25" s="15">
+        <v>43</v>
+      </c>
+      <c r="F25" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="G25" s="21"/>
+      <c r="H25" s="41"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" s="33"/>
+      <c r="E26" s="15">
+        <v>44</v>
+      </c>
+      <c r="F26" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="G26" s="21"/>
+      <c r="H26" s="41"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" s="33"/>
+      <c r="E27" s="15">
+        <v>45</v>
+      </c>
+      <c r="F27" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="G27" s="21"/>
+      <c r="H27" s="41"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" s="33"/>
+      <c r="E28" s="15">
+        <v>46</v>
+      </c>
+      <c r="F28" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="G28" s="21"/>
+      <c r="H28" s="41"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" s="33"/>
+      <c r="E29" s="15">
+        <v>47</v>
+      </c>
+      <c r="F29" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="G29" s="21"/>
+      <c r="H29" s="41"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30" s="33"/>
+      <c r="E30" s="15">
+        <v>48</v>
+      </c>
+      <c r="F30" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="G30" s="21"/>
+      <c r="H30" s="41"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B31" s="33"/>
+      <c r="E31" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="F31" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="G31" s="21"/>
+      <c r="H31" s="41"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32" s="33"/>
+      <c r="E32" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="F32" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="G32" s="21"/>
+      <c r="H32" s="41"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B33" s="33"/>
+      <c r="E33" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="F33" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="G33" s="21"/>
+      <c r="H33" s="41"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="16"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="17" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="18">
-        <v>0</v>
-      </c>
-      <c r="B3" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="E3" s="18">
-        <v>0</v>
-      </c>
-      <c r="F3" s="20" t="s">
+      <c r="B34" s="34"/>
+      <c r="E34" s="15">
+        <v>127</v>
+      </c>
+      <c r="F34" s="19" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="18">
-        <v>1</v>
-      </c>
-      <c r="B4" s="23"/>
-      <c r="E4" s="18">
-        <v>1</v>
-      </c>
-      <c r="F4" s="20"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="18">
-        <v>2</v>
-      </c>
-      <c r="B5" s="23"/>
-      <c r="E5" s="18">
-        <v>2</v>
-      </c>
-      <c r="F5" s="20"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="18">
-        <v>3</v>
-      </c>
-      <c r="B6" s="23"/>
-      <c r="E6" s="18">
-        <v>3</v>
-      </c>
-      <c r="F6" s="20"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="18">
-        <v>4</v>
-      </c>
-      <c r="B7" s="23"/>
-      <c r="E7" s="18">
-        <v>4</v>
-      </c>
-      <c r="F7" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H7" s="32" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="18">
-        <v>5</v>
-      </c>
-      <c r="B8" s="23"/>
-      <c r="E8" s="27">
-        <v>5</v>
-      </c>
-      <c r="F8" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="G8" s="38" t="s">
-        <v>41</v>
-      </c>
-      <c r="H8" s="35" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="18">
-        <v>6</v>
-      </c>
-      <c r="B9" s="23"/>
-      <c r="E9" s="27">
-        <v>6</v>
-      </c>
-      <c r="F9" s="30" t="s">
-        <v>40</v>
-      </c>
-      <c r="G9" s="33">
-        <v>1</v>
-      </c>
-      <c r="H9" s="36"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="18">
-        <v>7</v>
-      </c>
-      <c r="B10" s="23"/>
-      <c r="E10" s="27">
-        <v>7</v>
-      </c>
-      <c r="F10" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="G10" s="33"/>
-      <c r="H10" s="36"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="18">
-        <v>8</v>
-      </c>
-      <c r="B11" s="23"/>
-      <c r="E11" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="F11" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="G11" s="33"/>
-      <c r="H11" s="36"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="18">
-        <v>9</v>
-      </c>
-      <c r="B12" s="23"/>
-      <c r="E12" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="F12" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="G12" s="33"/>
-      <c r="H12" s="36"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="18">
-        <v>10</v>
-      </c>
-      <c r="B13" s="23"/>
-      <c r="E13" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="F13" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="G13" s="33"/>
-      <c r="H13" s="36"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="18">
-        <v>11</v>
-      </c>
-      <c r="B14" s="23"/>
-      <c r="E14" s="27">
-        <v>31</v>
-      </c>
-      <c r="F14" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="G14" s="34"/>
-      <c r="H14" s="37"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="B15" s="23"/>
-      <c r="E15" s="27">
-        <v>32</v>
-      </c>
-      <c r="F15" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="G15" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="H15" s="40" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16" s="23"/>
-      <c r="E16" s="27">
-        <v>34</v>
-      </c>
-      <c r="F16" s="30" t="s">
-        <v>40</v>
-      </c>
-      <c r="G16" s="39">
-        <v>1</v>
-      </c>
-      <c r="H16" s="41"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="B17" s="23"/>
-      <c r="E17" s="27">
-        <v>35</v>
-      </c>
-      <c r="F17" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="G17" s="33"/>
-      <c r="H17" s="41"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="B18" s="24"/>
-      <c r="E18" s="27">
-        <v>36</v>
-      </c>
-      <c r="F18" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="G18" s="33"/>
-      <c r="H18" s="41"/>
-    </row>
-    <row r="19" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="B19" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="E19" s="27">
-        <v>37</v>
-      </c>
-      <c r="F19" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="G19" s="33"/>
-      <c r="H19" s="41"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="B20" s="23"/>
-      <c r="E20" s="27">
-        <v>38</v>
-      </c>
-      <c r="F20" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="G20" s="33"/>
-      <c r="H20" s="41"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="B21" s="23"/>
-      <c r="E21" s="27">
-        <v>39</v>
-      </c>
-      <c r="F21" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="G21" s="33"/>
-      <c r="H21" s="41"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="B22" s="23"/>
-      <c r="E22" s="27">
-        <v>40</v>
-      </c>
-      <c r="F22" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="G22" s="33"/>
-      <c r="H22" s="41"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="B23" s="23"/>
-      <c r="E23" s="27">
-        <v>41</v>
-      </c>
-      <c r="F23" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="G23" s="33"/>
-      <c r="H23" s="41"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="B24" s="23"/>
-      <c r="E24" s="27">
-        <v>42</v>
-      </c>
-      <c r="F24" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="G24" s="33"/>
-      <c r="H24" s="41"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="B25" s="23"/>
-      <c r="E25" s="27">
-        <v>43</v>
-      </c>
-      <c r="F25" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="G25" s="33"/>
-      <c r="H25" s="41"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="B26" s="23"/>
-      <c r="E26" s="27">
-        <v>44</v>
-      </c>
-      <c r="F26" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="G26" s="33"/>
-      <c r="H26" s="41"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="B27" s="23"/>
-      <c r="E27" s="27">
-        <v>45</v>
-      </c>
-      <c r="F27" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="G27" s="33"/>
-      <c r="H27" s="41"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="B28" s="23"/>
-      <c r="E28" s="27">
-        <v>46</v>
-      </c>
-      <c r="F28" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="G28" s="33"/>
-      <c r="H28" s="41"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="B29" s="23"/>
-      <c r="E29" s="27">
-        <v>47</v>
-      </c>
-      <c r="F29" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="G29" s="33"/>
-      <c r="H29" s="41"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="B30" s="23"/>
-      <c r="E30" s="27">
-        <v>48</v>
-      </c>
-      <c r="F30" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="G30" s="33"/>
-      <c r="H30" s="41"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="B31" s="23"/>
-      <c r="E31" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="F31" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="G31" s="33"/>
-      <c r="H31" s="41"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="B32" s="23"/>
-      <c r="E32" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="F32" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="G32" s="33"/>
-      <c r="H32" s="41"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="B33" s="23"/>
-      <c r="E33" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="F33" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="G33" s="33"/>
-      <c r="H33" s="41"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="B34" s="24"/>
-      <c r="E34" s="27">
-        <v>127</v>
-      </c>
-      <c r="F34" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="G34" s="34"/>
+      <c r="G34" s="22"/>
       <c r="H34" s="42"/>
     </row>
   </sheetData>
@@ -1981,211 +2026,655 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="19"/>
-    <col min="2" max="2" width="10.7109375" style="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.28515625" style="19" customWidth="1"/>
-    <col min="4" max="4" width="22.5703125" style="19" customWidth="1"/>
-    <col min="5" max="5" width="175.7109375" style="19" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="19"/>
+    <col min="1" max="1" width="9.140625" style="13"/>
+    <col min="2" max="2" width="10.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.28515625" style="13" customWidth="1"/>
+    <col min="4" max="4" width="22.5703125" style="13" customWidth="1"/>
+    <col min="5" max="5" width="175.7109375" style="13" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="43"/>
-      <c r="B1" s="43" t="s">
+      <c r="A1" s="25"/>
+      <c r="B1" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="C1" s="43" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="43" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="43" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
+      <c r="E3" s="26" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="17" t="s">
+      <c r="B4" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="D3" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="E3" s="44" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="B4" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="D4" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="E4" s="17" t="s">
+      <c r="B5" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="E5" s="11" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="18" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="B5" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="D5" s="17" t="s">
+      <c r="B6" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="E5" s="17" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="s">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="B6" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="D6" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="E6" s="17" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="18" t="s">
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="B7" s="17"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
+      <c r="A9" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
+      <c r="A10" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
+      <c r="A11" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="21"/>
+      <c r="A12" s="14"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="21"/>
+      <c r="A13" s="14"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="21"/>
+      <c r="A14" s="14"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="21"/>
+      <c r="A15" s="14"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="21"/>
+      <c r="A16" s="14"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="21"/>
+      <c r="A17" s="14"/>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="21"/>
+      <c r="A18" s="14"/>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="21"/>
+      <c r="A19" s="14"/>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="21"/>
+      <c r="A20" s="14"/>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="21"/>
+      <c r="A21" s="14"/>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="21"/>
+      <c r="A22" s="14"/>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="21"/>
+      <c r="A23" s="14"/>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="21"/>
+      <c r="A24" s="14"/>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="21"/>
+      <c r="A25" s="14"/>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="21"/>
+      <c r="A26" s="14"/>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="21"/>
+      <c r="A27" s="14"/>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="21"/>
+      <c r="A28" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="13"/>
+    <col min="2" max="2" width="10.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.28515625" style="13" customWidth="1"/>
+    <col min="4" max="4" width="22.5703125" style="13" customWidth="1"/>
+    <col min="5" max="5" width="175.7109375" style="13" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="13"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="25"/>
+      <c r="B1" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="E3" s="26" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="14"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="14"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="14"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="14"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="14"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="14"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="14"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="14"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="14"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="14"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="14"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="14"/>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="14"/>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="14"/>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="14"/>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="14"/>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="14"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="13"/>
+    <col min="2" max="2" width="10.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.28515625" style="13" customWidth="1"/>
+    <col min="4" max="4" width="25.140625" style="13" customWidth="1"/>
+    <col min="5" max="5" width="196.140625" style="13" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="13"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="25"/>
+      <c r="B1" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="E3" s="26" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="E7" s="47" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="D8" s="45" t="s">
+        <v>72</v>
+      </c>
+      <c r="E8" s="46"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="14"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="14"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="14"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="14"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="14"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="14"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="14"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="14"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="14"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="14"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="14"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="14"/>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="14"/>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="14"/>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="14"/>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="14"/>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="14"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D8:E8"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>